<commit_message>
# changed from taqTT25 to taqTT26
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\MyProjects\kinmodre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44922F76-3A57-441B-9334-4883CFC8792A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C1F32F-BA49-4F3D-ABEE-72D3DA771DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
   <si>
     <t>Model Name</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>Ambel et al. 2025. UniKin2 – A Universal, Pan-Reactome Kinetic Model. International Journal of Research in Medical and Clinical Science 3(2): 77-80.</t>
+  </si>
+  <si>
+    <t>spnLHP26</t>
   </si>
 </sst>
 </file>
@@ -869,7 +872,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1322,11 +1325,26 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="4">
+        <v>2026</v>
+      </c>
       <c r="C20" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>58</v>
+      </c>
+      <c r="E20" s="4">
+        <v>836</v>
+      </c>
+      <c r="F20" s="4">
+        <v>460</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1014</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
+ added stheVS26 kinetic model
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C1F32F-BA49-4F3D-ABEE-72D3DA771DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8C266D-3232-4193-A18D-F3C8B65AF182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="79">
   <si>
     <t>Model Name</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>spnLHP26</t>
+  </si>
+  <si>
+    <t>stheVS26</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -520,19 +523,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -872,21 +866,21 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="6.54296875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="39.90625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" style="4" customWidth="1"/>
-    <col min="5" max="7" width="15.1796875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="130.1796875" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="7"/>
+    <col min="1" max="1" width="18.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.90625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.1796875" style="2" customWidth="1"/>
+    <col min="5" max="7" width="15.1796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="130.1796875" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -934,7 +928,7 @@
       <c r="G2" s="2">
         <v>310</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -960,7 +954,7 @@
       <c r="G3" s="2">
         <v>310</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -986,7 +980,7 @@
       <c r="G4" s="2">
         <v>533</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1012,7 +1006,7 @@
       <c r="G5" s="2">
         <v>68</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1038,7 +1032,7 @@
       <c r="G6" s="2">
         <v>231</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1064,7 +1058,7 @@
       <c r="G7" s="2">
         <v>302</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1090,7 +1084,7 @@
       <c r="G8" s="2">
         <v>1624</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1116,7 +1110,7 @@
       <c r="G9" s="2">
         <v>1801</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1142,7 +1136,7 @@
       <c r="G10" s="2">
         <v>931</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1168,7 +1162,7 @@
       <c r="G11" s="2">
         <v>1681</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1194,67 +1188,67 @@
       <c r="G12" s="2">
         <v>1388</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>2025</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="2">
         <v>1300</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="2">
         <v>650</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="2">
         <v>1053</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="2">
         <v>2025</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="2">
         <v>168</v>
       </c>
       <c r="E14" s="2">
         <v>1565</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="2">
         <v>679</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="2">
         <v>1554</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="2">
         <v>2025</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1263,166 +1257,181 @@
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="2">
         <v>9420</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="2">
         <v>9420</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="2">
         <v>30669</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2026</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="E17" s="2">
+        <v>336</v>
+      </c>
+      <c r="F17" s="2">
+        <v>400</v>
+      </c>
+      <c r="G17" s="2">
+        <v>322</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="2">
         <v>2026</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <v>768</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="2">
         <v>276</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="2">
         <v>1288</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="2">
         <v>2026</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2">
         <v>836</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="2">
         <v>460</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="2">
         <v>1014</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="2">
         <v>2026</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="2">
         <v>1552</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="2">
         <v>431</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="2">
         <v>1059</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
+ added kinetic model lcaKKNC26
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9823AC7C-572E-47EE-9210-66467A2FF37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5CE642-A88E-4CDF-B158-4E92BB7EC9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
   <si>
     <t>Model Name</t>
   </si>
@@ -445,12 +445,45 @@
   <si>
     <t>hinSAH26</t>
   </si>
+  <si>
+    <t>Bifidobacterium breve</t>
+  </si>
+  <si>
+    <t>DSM 20213</t>
+  </si>
+  <si>
+    <t>SEZ13</t>
+  </si>
+  <si>
+    <t>Bifidobacterium longum</t>
+  </si>
+  <si>
+    <t>Streptococcus equi subsp. Zooepidemicus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JCM 1217</t>
+  </si>
+  <si>
+    <t>Clostridioides difficile</t>
+  </si>
+  <si>
+    <t>R20291</t>
+  </si>
+  <si>
+    <t>Corynebacterium glutamicum</t>
+  </si>
+  <si>
+    <t>ATCC 13032</t>
+  </si>
+  <si>
+    <t>lcaKKNC26</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,6 +508,13 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -526,10 +566,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -865,11 +905,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5584041-A284-4063-80B3-FA0C9EAD7AB9}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -879,8 +919,8 @@
     <col min="3" max="3" width="39.90625" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.1796875" style="2" customWidth="1"/>
     <col min="5" max="7" width="15.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="130.1796875" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="5"/>
+    <col min="8" max="8" width="130.1796875" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.35">
@@ -931,7 +971,7 @@
       <c r="G2" s="2">
         <v>310</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -957,7 +997,7 @@
       <c r="G3" s="2">
         <v>310</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -983,7 +1023,7 @@
       <c r="G4" s="2">
         <v>533</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1009,7 +1049,7 @@
       <c r="G5" s="2">
         <v>68</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1035,7 +1075,7 @@
       <c r="G6" s="2">
         <v>231</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1061,7 +1101,7 @@
       <c r="G7" s="2">
         <v>302</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1087,7 +1127,7 @@
       <c r="G8" s="2">
         <v>1624</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1113,7 +1153,7 @@
       <c r="G9" s="2">
         <v>1801</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1139,7 +1179,7 @@
       <c r="G10" s="2">
         <v>931</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1165,7 +1205,7 @@
       <c r="G11" s="2">
         <v>1681</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1191,7 +1231,7 @@
       <c r="G12" s="2">
         <v>1388</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1217,7 +1257,7 @@
       <c r="G13" s="2">
         <v>1053</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1243,7 +1283,7 @@
       <c r="G14" s="2">
         <v>1554</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1269,18 +1309,32 @@
       <c r="G15" s="2">
         <v>30669</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2026</v>
+      </c>
       <c r="C16" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="2">
+        <v>677</v>
+      </c>
+      <c r="F16" s="2">
+        <v>356</v>
+      </c>
+      <c r="G16" s="2">
+        <v>846</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
@@ -1451,6 +1505,46 @@
       </c>
       <c r="D28" s="2" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C29" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C30" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C32" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C33" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ added GRN for lcaKKNC26
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5CE642-A88E-4CDF-B158-4E92BB7EC9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A631D9C-68C1-4ECF-8587-851176CCF789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -908,8 +908,8 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
# sorted out errors for KM ddsAAR26
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\MyProjects\kinmodre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71BA510-064F-4E4B-AF2D-00DFEE7034A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AAD125-781C-44CE-B52F-59BAA3E996C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -920,8 +920,8 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1385,13 +1385,13 @@
         <v>54</v>
       </c>
       <c r="E18" s="2">
-        <v>768</v>
+        <v>573</v>
       </c>
       <c r="F18" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G18" s="2">
-        <v>1288</v>
+        <v>701</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
+ added publication for stjDNV26
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C251B4-C16C-4261-9EB6-30A39591634A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219560BF-1F88-4ED2-BED4-F5EFB6C75D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
   <si>
     <t>Model Name</t>
   </si>
@@ -495,6 +495,12 @@
   </si>
   <si>
     <t>cglPS26</t>
+  </si>
+  <si>
+    <t>Tay et al. 2026. Ab Initio Whole Cell Kinetic Model of Thermus aquaticus Y51MC23 (taqTT26). Scholastic Medical Sciences 3(1): 01-04.</t>
+  </si>
+  <si>
+    <t>Nanthakumarvani et al. 2026. Ab Initio Whole Cell Kinetic Model of Streptococcus salivarius JIM8777 (stjDNV26). American Journal of Pathology &amp; Research 5(1): 1-4.</t>
   </si>
 </sst>
 </file>
@@ -572,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -588,6 +594,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,8 +935,8 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1354,7 +1363,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>77</v>
       </c>
@@ -1377,7 +1386,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>95</v>
       </c>
@@ -1422,8 +1431,11 @@
       <c r="G19" s="2">
         <v>842</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>76</v>
       </c>
@@ -1446,7 +1458,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>78</v>
       </c>
@@ -1469,7 +1481,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>90</v>
       </c>
@@ -1492,7 +1504,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>73</v>
       </c>
@@ -1514,8 +1526,11 @@
       <c r="G23" s="2">
         <v>1059</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>91</v>
       </c>
@@ -1538,99 +1553,99 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C25" s="3" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2026</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1153</v>
+      </c>
+      <c r="F25" s="2">
+        <v>444</v>
+      </c>
+      <c r="G25" s="2">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C26" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C26" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C28" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C29" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C30" s="5" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C31" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C31" s="5" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C32" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C32" s="5" t="s">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C33" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C33" s="5" t="s">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C34" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="2">
-        <v>2026</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34" s="2">
-        <v>1153</v>
-      </c>
-      <c r="F34" s="2">
-        <v>444</v>
-      </c>
-      <c r="G34" s="2">
-        <v>986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ added paper for spnLHP26
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\MyProjects\kinmodre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DCFED2-64B1-4326-93B8-D77F7336ED6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE5CA7F-34DC-4965-B94D-1627795C45EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
   <si>
     <t>Model Name</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t>smuLA26</t>
+  </si>
+  <si>
+    <t>Perumal et al. 2026. Ab Initio Whole Cell Kinetic Model of Streptococcus pneumoniae NCTC 7465 (spnLHP26). Clareus Scientific Medical Sciences 3(1): 02-07.</t>
+  </si>
+  <si>
+    <t>RajKumar et al. 2026. Ab Initio Whole Cell Kinetic Model of Desulfovibrio desulfuricans L4 (ddsAAR26). Journal of Clinical Immunology &amp; Microbiology 7(1): 1-5.</t>
   </si>
 </sst>
 </file>
@@ -581,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -598,9 +604,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,8 +945,8 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1389,7 +1396,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
@@ -1410,6 +1417,9 @@
       </c>
       <c r="G18" s="2">
         <v>701</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="31" x14ac:dyDescent="0.35">
@@ -1459,6 +1469,9 @@
       </c>
       <c r="G20" s="2">
         <v>1014</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
+ added caccSM26 paper
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE5CA7F-34DC-4965-B94D-1627795C45EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310A7275-87C3-4648-8D66-BCC0546A85B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
   <si>
     <t>Model Name</t>
   </si>
@@ -510,6 +510,9 @@
   </si>
   <si>
     <t>RajKumar et al. 2026. Ab Initio Whole Cell Kinetic Model of Desulfovibrio desulfuricans L4 (ddsAAR26). Journal of Clinical Immunology &amp; Microbiology 7(1): 1-5.</t>
+  </si>
+  <si>
+    <t>Murugesu et al. 2026. Ab Initio Whole Cell Kinetic Model of Corynebacterium accolens DSM 44278 (caccSM26). EC Clinical and Medical Case Reports 9(2): 01-06.</t>
   </si>
 </sst>
 </file>
@@ -946,7 +949,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1546,7 +1549,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>91</v>
       </c>
@@ -1567,6 +1570,9 @@
       </c>
       <c r="G24" s="2">
         <v>1097</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
+ added publication for pdiMLD26
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310A7275-87C3-4648-8D66-BCC0546A85B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810008EC-7CE5-4001-A087-CC02D7CF04CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <t>Model Name</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t>Murugesu et al. 2026. Ab Initio Whole Cell Kinetic Model of Corynebacterium accolens DSM 44278 (caccSM26). EC Clinical and Medical Case Reports 9(2): 01-06.</t>
+  </si>
+  <si>
+    <t>Dhinakaran et al. 2026. Ab Initio Whole Cell Kinetic Model of Parabacteroides distasonis APCS2/PD (pdiMLD26). Acta Scientific Medical Science 10(2): 52-56.</t>
   </si>
 </sst>
 </file>
@@ -948,8 +951,8 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1500,7 +1503,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>90</v>
       </c>
@@ -1521,6 +1524,9 @@
       </c>
       <c r="G22" s="2">
         <v>703</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
+ added publication for lcaKKNC26
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810008EC-7CE5-4001-A087-CC02D7CF04CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E44623-3939-4F77-9742-F6A74345E4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
   <si>
     <t>Model Name</t>
   </si>
@@ -516,6 +516,9 @@
   </si>
   <si>
     <t>Dhinakaran et al. 2026. Ab Initio Whole Cell Kinetic Model of Parabacteroides distasonis APCS2/PD (pdiMLD26). Acta Scientific Medical Science 10(2): 52-56.</t>
+  </si>
+  <si>
+    <t>Kang et al. 2026. Ab Initio Whole Cell Kinetic Model of Lacticaseibacillus paracasei subspecies paracasei NTU 101 (lcaKKNC26). Acta Scientific Microbiology 9(2): 03-08.</t>
   </si>
 </sst>
 </file>
@@ -951,8 +954,8 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1356,7 +1359,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>89</v>
       </c>
@@ -1377,6 +1380,9 @@
       </c>
       <c r="G16" s="2">
         <v>846</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
+ added publication for stheVS26
</commit_message>
<xml_diff>
--- a/List of Kinetic Models.xlsx
+++ b/List of Kinetic Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\MyProjects\kinmodre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E44623-3939-4F77-9742-F6A74345E4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC26B776-21EB-404E-A452-C70B8688A1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A48245FD-6B6A-497E-8B16-C1CADEA3146F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="106">
   <si>
     <t>Model Name</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>Kang et al. 2026. Ab Initio Whole Cell Kinetic Model of Lacticaseibacillus paracasei subspecies paracasei NTU 101 (lcaKKNC26). Acta Scientific Microbiology 9(2): 03-08.</t>
+  </si>
+  <si>
+    <t>Verma et al. 2026. Ab Initio Whole Cell Kinetic Model of Streptococcus thermophilus STH_CIRM_65 (stheVS26). Acta Scientific Nutritional Health 10(2): 43-47.</t>
   </si>
 </sst>
 </file>
@@ -955,7 +958,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1385,7 +1388,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>77</v>
       </c>
@@ -1406,6 +1409,9 @@
       </c>
       <c r="G17" s="2">
         <v>322</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="31" x14ac:dyDescent="0.35">

</xml_diff>